<commit_message>
Added all_tanks sights for AB/RB Floppa, added RU version
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AB" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="AP" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="APDS" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="LASER" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="ALL_TANKS" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16562" uniqueCount="1893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16583" uniqueCount="1894">
   <si>
     <t xml:space="preserve">uk_centurion_mk_5_avre_era</t>
   </si>
@@ -5706,6 +5707,9 @@
   </si>
   <si>
     <t xml:space="preserve">0.533, 0.730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all_tanks</t>
   </si>
 </sst>
 </file>
@@ -5873,11 +5877,11 @@
   </sheetPr>
   <dimension ref="A1:I789"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A659" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A716" activeCellId="0" sqref="A716"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A716" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G764" activeCellId="0" sqref="G764"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
   </cols>
@@ -21639,7 +21643,7 @@
       <selection pane="topLeft" activeCell="A716" activeCellId="0" sqref="A716"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
   </cols>
@@ -38094,10 +38098,10 @@
   <dimension ref="A1:I892"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A184" activeCellId="0" sqref="A184"/>
+      <selection pane="topLeft" activeCell="D185" activeCellId="0" sqref="D185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
   </cols>
@@ -61821,7 +61825,7 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A185" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A185" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A231" activeCellId="0" sqref="A231"/>
     </sheetView>
   </sheetViews>
@@ -72260,4 +72264,182 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>622</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>982</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>983</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>984</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>986</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>